<commit_message>
Fixed bug in surface tension code, making the surface tension always 0 self.pos_grid --> self.pos_grid_gpu
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAD6F36-5627-45CF-98EC-E3768A9B040F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882504E3-7FC6-4168-AD15-520DEBC6424B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5235" windowWidth="29040" windowHeight="15720" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
+    <workbookView xWindow="-28425" yWindow="5745" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Spring constant (k)</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>Damping coefficient (c)</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
 </sst>
 </file>
@@ -464,7 +467,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -556,7 +559,7 @@
         <v>10000</v>
       </c>
       <c r="D3">
-        <v>10000</v>
+        <v>0.5</v>
       </c>
       <c r="E3">
         <v>0.05</v>
@@ -586,10 +589,10 @@
         <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>10000</v>
+        <v>50000</v>
       </c>
       <c r="D4" s="2">
-        <v>10000</v>
+        <v>0.5</v>
       </c>
       <c r="E4" s="2">
         <v>0.05</v>
@@ -604,10 +607,10 @@
         <v>150000000</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="J4" s="2">
-        <v>1E-4</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K4" s="2">
         <v>-9.81</v>

</xml_diff>

<commit_message>
Fixed bug in hookes_law that uses wrong velocity. Detected during report writing
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{882504E3-7FC6-4168-AD15-520DEBC6424B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0FCD7CE-99FB-4F30-B241-D61580087769}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28425" yWindow="5745" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -559,7 +559,7 @@
         <v>10000</v>
       </c>
       <c r="D3">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="E3">
         <v>0.05</v>
@@ -592,7 +592,7 @@
         <v>50000</v>
       </c>
       <c r="D4" s="2">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="E4" s="2">
         <v>0.05</v>

</xml_diff>

<commit_message>
Added comments to Output_Centre.py
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4982B0E6-3774-401E-92D8-ECF482937E54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86255A24-A61B-46A2-A274-908C2B172E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28425" yWindow="5745" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
+    <workbookView xWindow="-27990" yWindow="6180" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,7 +92,7 @@
     <t>Damping coefficient (c)</t>
   </si>
   <si>
-    <t>500</t>
+    <t>150</t>
   </si>
 </sst>
 </file>
@@ -474,7 +474,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -596,13 +596,13 @@
         <v>10</v>
       </c>
       <c r="C4" s="2">
+        <v>10</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0.01</v>
+      </c>
+      <c r="E4">
         <v>0.05</v>
-      </c>
-      <c r="D4" s="7">
-        <v>3.2800000000000003E-2</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
       </c>
       <c r="F4" s="2">
         <v>10</v>

</xml_diff>

<commit_message>
Created basic CPU implementation by converting GPU code to numpy from cupy Updated Settings.xlsx and Settings_hub.py to allow user to change compute device
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86255A24-A61B-46A2-A274-908C2B172E4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6D4826-8CDE-4FFD-AF09-D95F5F8DF08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27990" yWindow="6180" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Spring constant (k)</t>
   </si>
@@ -92,7 +92,13 @@
     <t>Damping coefficient (c)</t>
   </si>
   <si>
-    <t>150</t>
+    <t>GPU Compute</t>
+  </si>
+  <si>
+    <t>bool</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -471,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D8172A-B57A-44AD-875F-052277048E07}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,9 +496,10 @@
     <col min="9" max="9" width="7.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -523,8 +530,11 @@
       <c r="K1" t="s">
         <v>11</v>
       </c>
+      <c r="L1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" t="s">
         <v>5</v>
@@ -556,8 +566,11 @@
       <c r="K2" t="s">
         <v>6</v>
       </c>
+      <c r="L2" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>8</v>
@@ -589,8 +602,11 @@
       <c r="K3">
         <v>-9.81</v>
       </c>
+      <c r="L3" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>10</v>
@@ -599,7 +615,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="7">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E4">
         <v>0.05</v>
@@ -614,13 +630,16 @@
         <v>150000000</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J4" s="2">
         <v>1E-4</v>
       </c>
       <c r="K4" s="2">
         <v>-9.81</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated all unit tests to be aware of CPU implementation
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D6D4826-8CDE-4FFD-AF09-D95F5F8DF08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C3D8F1-4082-49A1-A2F7-0A28D166172C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27990" yWindow="6180" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>Spring constant (k)</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>bool</t>
-  </si>
-  <si>
-    <t>False</t>
   </si>
 </sst>
 </file>
@@ -480,7 +477,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -615,7 +612,7 @@
         <v>10</v>
       </c>
       <c r="D4" s="7">
-        <v>0.02</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="E4">
         <v>0.05</v>
@@ -639,7 +636,7 @@
         <v>-9.81</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Due to instability in Verlet as an emergency Euler Richardson has been added
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C3D8F1-4082-49A1-A2F7-0A28D166172C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0F0E53-2B65-40A1-A1B9-2364267EE438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27990" yWindow="6180" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
+    <workbookView xWindow="-27120" yWindow="7050" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t>Spring constant (k)</t>
   </si>
@@ -96,14 +96,27 @@
   </si>
   <si>
     <t>bool</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Numerical Method</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>string (ER or V)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -154,7 +167,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -474,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D8172A-B57A-44AD-875F-052277048E07}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,9 +507,10 @@
     <col min="10" max="10" width="16.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.77734375" customWidth="1"/>
+    <col min="13" max="13" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -530,8 +544,11 @@
       <c r="L1" t="s">
         <v>18</v>
       </c>
+      <c r="M1" t="s">
+        <v>21</v>
+      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" t="s">
         <v>5</v>
@@ -566,14 +583,17 @@
       <c r="L2" t="s">
         <v>19</v>
       </c>
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3">
-        <v>10000</v>
+        <v>10</v>
       </c>
       <c r="D3" s="6">
         <v>7.2800000000000004E-2</v>
@@ -602,17 +622,20 @@
       <c r="L3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="M3" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>10</v>
       </c>
       <c r="C4" s="2">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="D4" s="7">
-        <v>5.0000000000000001E-4</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="E4">
         <v>0.05</v>
@@ -627,16 +650,19 @@
         <v>150000000</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="J4" s="2">
-        <v>1E-4</v>
+        <v>5.0000000000000002E-5</v>
       </c>
       <c r="K4" s="2">
         <v>-9.81</v>
       </c>
       <c r="L4" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="M4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added pool resizing in Settings_hub.py and Settings.xlsx. Elastic energy still increases, even with a changed integrator, indicating another problem
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0F0E53-2B65-40A1-A1B9-2364267EE438}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE51016D-DBFE-48E9-8F46-CC8AD0E514E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27120" yWindow="7050" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
   <si>
     <t>Spring constant (k)</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>string (ER or V)</t>
+  </si>
+  <si>
+    <t>x size</t>
+  </si>
+  <si>
+    <t>y size</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D8172A-B57A-44AD-875F-052277048E07}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -510,7 +516,7 @@
     <col min="13" max="13" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
@@ -547,8 +553,14 @@
       <c r="M1" t="s">
         <v>21</v>
       </c>
+      <c r="N1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O1" t="s">
+        <v>25</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" t="s">
         <v>5</v>
@@ -586,8 +598,14 @@
       <c r="M2" t="s">
         <v>23</v>
       </c>
+      <c r="N2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>8</v>
@@ -625,8 +643,14 @@
       <c r="M3" t="s">
         <v>22</v>
       </c>
+      <c r="N3">
+        <v>100</v>
+      </c>
+      <c r="O3">
+        <v>100</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>10</v>
@@ -663,6 +687,12 @@
       </c>
       <c r="M4" t="s">
         <v>22</v>
+      </c>
+      <c r="N4">
+        <v>10000</v>
+      </c>
+      <c r="O4">
+        <v>10000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed graph formatting Fixed minor arrays with a low effort method (Now just 2 timestep arrays)
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD16FFE2-45EC-4000-B931-07B33514ED63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E1B1D6-D786-4EC2-8931-BC7CBD2B98F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-27120" yWindow="7050" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>Spring constant (k)</t>
   </si>
   <si>
-    <t>Surface tension coefficient (sigma)</t>
-  </si>
-  <si>
     <t>Surface mass (pool_mass)</t>
   </si>
   <si>
@@ -98,32 +95,31 @@
     <t>bool</t>
   </si>
   <si>
+    <t>Numerical Method</t>
+  </si>
+  <si>
+    <t>ER</t>
+  </si>
+  <si>
+    <t>string (ER or V)</t>
+  </si>
+  <si>
+    <t>x size</t>
+  </si>
+  <si>
+    <t>y size</t>
+  </si>
+  <si>
     <t>200</t>
   </si>
   <si>
-    <t>Numerical Method</t>
-  </si>
-  <si>
-    <t>ER</t>
-  </si>
-  <si>
-    <t>string (ER or V)</t>
-  </si>
-  <si>
-    <t>x size</t>
-  </si>
-  <si>
-    <t>y size</t>
+    <t>Surface tension coefficient (sigma) (Causes stability issues if turned up above 0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="165" formatCode="0.000"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -172,12 +168,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,7 +492,7 @@
   <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -504,7 +500,7 @@
     <col min="1" max="1" width="23.77734375" customWidth="1"/>
     <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="56.88671875" bestFit="1" customWidth="1"/>
@@ -517,104 +513,104 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>12</v>
+      <c r="A1" s="6" t="s">
+        <v>11</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="F1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
-        <v>4</v>
-      </c>
-      <c r="K1" t="s">
-        <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>18</v>
-      </c>
       <c r="M1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="N1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="O1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
+      <c r="A2" s="6"/>
       <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>7</v>
-      </c>
       <c r="H2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="N2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="O2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="8"/>
+      <c r="A3" s="6"/>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
-      <c r="D3" s="6">
-        <v>7.2800000000000004E-2</v>
+      <c r="D3" s="7">
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0.05</v>
@@ -623,13 +619,13 @@
         <v>10</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H3" s="4">
         <v>150000000</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3">
         <v>1E-4</v>
@@ -638,10 +634,10 @@
         <v>-9.81</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N3">
         <v>100</v>
@@ -651,15 +647,15 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="8"/>
+      <c r="A4" s="6"/>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2">
         <v>10000</v>
       </c>
-      <c r="D4" s="7">
-        <v>3.0000000000000001E-3</v>
+      <c r="D4" s="8">
+        <v>0</v>
       </c>
       <c r="E4">
         <v>0.05</v>
@@ -668,13 +664,13 @@
         <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" s="5">
         <v>150000000</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="J4" s="2">
         <v>5.0000000000000002E-5</v>
@@ -683,16 +679,16 @@
         <v>-9.81</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="M4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="N4">
-        <v>100000</v>
+        <v>100</v>
       </c>
       <c r="O4">
-        <v>100000</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix numba error in Output_Centre.py
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E1B1D6-D786-4EC2-8931-BC7CBD2B98F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F85B452-065A-4433-A4F7-C1C86230C0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27120" yWindow="7050" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
+    <workbookView xWindow="-26685" yWindow="7485" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
   <si>
     <t>Spring constant (k)</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Surface tension coefficient (sigma) (Causes stability issues if turned up above 0)</t>
+  </si>
+  <si>
+    <t>V</t>
   </si>
 </sst>
 </file>
@@ -168,12 +171,12 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -491,8 +494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D8172A-B57A-44AD-875F-052277048E07}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,7 +516,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
       <c r="C1" t="s">
@@ -557,7 +560,7 @@
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="6"/>
+      <c r="A2" s="8"/>
       <c r="B2" t="s">
         <v>4</v>
       </c>
@@ -602,14 +605,14 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
+      <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>7</v>
       </c>
       <c r="C3">
         <v>10</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D3" s="6">
         <v>0</v>
       </c>
       <c r="E3">
@@ -647,14 +650,14 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="6"/>
+      <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="2">
         <v>10000</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>0</v>
       </c>
       <c r="E4">
@@ -682,7 +685,7 @@
         <v>8</v>
       </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="N4">
         <v>100</v>

</xml_diff>

<commit_message>
Added setting for custom shape
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F85B452-065A-4433-A4F7-C1C86230C0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D391B90-EEF1-49D2-864F-C438459250DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26685" yWindow="7485" windowWidth="23010" windowHeight="12105" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
+    <workbookView xWindow="-28920" yWindow="5235" windowWidth="29040" windowHeight="15720" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>Spring constant (k)</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>Custom Shape?</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
 </sst>
 </file>
@@ -492,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D8172A-B57A-44AD-875F-052277048E07}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -513,9 +519,10 @@
     <col min="11" max="11" width="26.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.77734375" customWidth="1"/>
     <col min="13" max="13" width="17.21875" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>11</v>
       </c>
@@ -558,8 +565,11 @@
       <c r="O1" t="s">
         <v>23</v>
       </c>
+      <c r="P1" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="8"/>
       <c r="B2" t="s">
         <v>4</v>
@@ -603,8 +613,11 @@
       <c r="O2" t="s">
         <v>5</v>
       </c>
+      <c r="P2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="8"/>
       <c r="B3" t="s">
         <v>7</v>
@@ -648,8 +661,11 @@
       <c r="O3">
         <v>100</v>
       </c>
+      <c r="P3" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="8"/>
       <c r="B4" t="s">
         <v>9</v>
@@ -692,6 +708,9 @@
       </c>
       <c r="O4">
         <v>100</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hotfix for shape setting, fixed column in excel sheet loaded
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D391B90-EEF1-49D2-864F-C438459250DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA75D69C-C48F-4BD3-8753-B9AB50121085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5235" windowWidth="29040" windowHeight="15720" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="23016" windowHeight="12108" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,7 +710,7 @@
         <v>100</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed errors taking the wrong axis for length
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA75D69C-C48F-4BD3-8753-B9AB50121085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C15A3A-7C78-4A70-A86B-B04464CE0B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2688" yWindow="2688" windowWidth="23016" windowHeight="12108" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D8172A-B57A-44AD-875F-052277048E07}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,7 +710,7 @@
         <v>100</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Hotfix for shape setting, fixed column in excel sheet loaded"
This reverts commit 5b2674060c785798dff3246105c530cd540c0c73.
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA75D69C-C48F-4BD3-8753-B9AB50121085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D391B90-EEF1-49D2-864F-C438459250DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="23016" windowHeight="12108" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
+    <workbookView xWindow="-28920" yWindow="5235" windowWidth="29040" windowHeight="15720" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,7 +710,7 @@
         <v>100</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>28</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bugs with minor arrays
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D391B90-EEF1-49D2-864F-C438459250DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFEB840-13D4-436B-AD8F-76E84E1C3946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5235" windowWidth="29040" windowHeight="15720" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
+    <workbookView xWindow="-28905" yWindow="5355" windowWidth="14610" windowHeight="15585" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -110,9 +110,6 @@
     <t>y size</t>
   </si>
   <si>
-    <t>200</t>
-  </si>
-  <si>
     <t>Surface tension coefficient (sigma) (Causes stability issues if turned up above 0)</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>False</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D8172A-B57A-44AD-875F-052277048E07}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -530,7 +530,7 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E1" t="s">
         <v>16</v>
@@ -566,7 +566,7 @@
         <v>23</v>
       </c>
       <c r="P1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
@@ -662,7 +662,7 @@
         <v>100</v>
       </c>
       <c r="P3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.3">
@@ -683,13 +683,13 @@
         <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="H4" s="5">
         <v>150000000</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="J4" s="2">
         <v>5.0000000000000002E-5</v>
@@ -701,7 +701,7 @@
         <v>8</v>
       </c>
       <c r="M4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="N4">
         <v>100</v>

</xml_diff>

<commit_message>
Fixed CPU_Calculation_Centre.py for Minor arrays
</commit_message>
<xml_diff>
--- a/Settings/Settings.xlsx
+++ b/Settings/Settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Waveular\Settings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFEB840-13D4-436B-AD8F-76E84E1C3946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB57D21-BE4E-43E6-81AE-E2CB0CBA1F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="5355" windowWidth="14610" windowHeight="15585" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
+    <workbookView xWindow="-28920" yWindow="5235" windowWidth="29040" windowHeight="15720" xr2:uid="{7393ABB7-F9E9-45B7-8ABE-C15D8C3A34DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -122,7 +122,7 @@
     <t>False</t>
   </si>
   <si>
-    <t>1</t>
+    <t>150</t>
   </si>
 </sst>
 </file>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D8172A-B57A-44AD-875F-052277048E07}">
   <dimension ref="A1:P4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -623,7 +623,7 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="D3" s="6">
         <v>0</v>
@@ -683,7 +683,7 @@
         <v>10</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="H4" s="5">
         <v>150000000</v>
@@ -698,7 +698,7 @@
         <v>-9.81</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="M4" t="s">
         <v>25</v>
@@ -710,7 +710,7 @@
         <v>100</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>